<commit_message>
Add EC & BVA tables only last table to be completed added tests in TestLink (and gen doc) changed test name
</commit_message>
<xml_diff>
--- a/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D18F04-48D5-4275-BBE5-09AE99554378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455CE643-3EF9-4531-829A-61E6D2258557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="131">
   <si>
     <t>VVSS, Info Romana, 2023-2024</t>
   </si>
@@ -166,38 +166,10 @@
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
   <si>
-    <t>Un cinefil doreşte să îşi dezvolte un program pentru gestionarea filmelor din colecţia personală. Programul va permite următoarele operaţii:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>F01.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> adăugarea unui film nou (titlu, regizor, an aparitie, actori, categorie, cuvinte cheie);</t>
-    </r>
-  </si>
-  <si>
     <t>Observații</t>
   </si>
   <si>
     <t xml:space="preserve">1. La proiectarea TCs se consideră o metodă care poate avea următoarea semnătură: </t>
-  </si>
-  <si>
-    <t>addMovie(String title, String director, int year, List&lt;String&gt; actors, String category, List&lt;String&gt; keywords): void</t>
   </si>
   <si>
     <t>2. Metoda este definită la nivelul repository, service sau ui.</t>
@@ -328,39 +300,12 @@
     <t>output data</t>
   </si>
   <si>
-    <t>titlu</t>
-  </si>
-  <si>
-    <t>regizor</t>
-  </si>
-  <si>
-    <t>an aparitie</t>
-  </si>
-  <si>
-    <t>actori</t>
-  </si>
-  <si>
-    <t>categorie</t>
-  </si>
-  <si>
-    <t>cuvinte cheie</t>
-  </si>
-  <si>
     <t>expected</t>
   </si>
   <si>
     <t>"Movie Title"</t>
   </si>
   <si>
-    <t>Actor1, Actor2</t>
-  </si>
-  <si>
-    <t>keyword1, keyword2</t>
-  </si>
-  <si>
-    <t>2,3,2</t>
-  </si>
-  <si>
     <t>record added</t>
   </si>
   <si>
@@ -376,18 +321,9 @@
     <t>""</t>
   </si>
   <si>
-    <t>..</t>
-  </si>
-  <si>
-    <t>201q</t>
-  </si>
-  <si>
     <t>Error message-? Compiler checked</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -415,19 +351,7 @@
     <t>expected result</t>
   </si>
   <si>
-    <t>TC3_EC</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>"M"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Director1, Director 2</t>
-  </si>
-  <si>
-    <t>Drama</t>
   </si>
   <si>
     <t>"M…123"</t>
@@ -544,9 +468,6 @@
     <t>Șofran Daniel</t>
   </si>
   <si>
-    <t>1. Managementul taskurilor</t>
-  </si>
-  <si>
     <t>data este existenta</t>
   </si>
   <si>
@@ -593,6 +514,114 @@
   </si>
   <si>
     <t>1, 6</t>
+  </si>
+  <si>
+    <t>noTimeDate</t>
+  </si>
+  <si>
+    <t>timpul e valid, 00:00&lt;t&lt;23:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data e valida, 01.01.1970 &lt;date&lt; 31.12.9999  </t>
+  </si>
+  <si>
+    <t>01. date=31.12.1969</t>
+  </si>
+  <si>
+    <t>02. date=01.01.1970</t>
+  </si>
+  <si>
+    <t>03. date=02.01.1970</t>
+  </si>
+  <si>
+    <t>04. date=30.12.9999</t>
+  </si>
+  <si>
+    <t>05. date=31.12.9999</t>
+  </si>
+  <si>
+    <t>06. date=01.01.10000</t>
+  </si>
+  <si>
+    <t>07. time=00:-1</t>
+  </si>
+  <si>
+    <t>08. time=00:00</t>
+  </si>
+  <si>
+    <t>09. time=00:01</t>
+  </si>
+  <si>
+    <t>10. time=23:58</t>
+  </si>
+  <si>
+    <t>11. time=23:59</t>
+  </si>
+  <si>
+    <t>12. time=24:00</t>
+  </si>
+  <si>
+    <t>13. time=23:60</t>
+  </si>
+  <si>
+    <t>`10-30`</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>23:5a</t>
+  </si>
+  <si>
+    <t>public static Date getDateMergedWithTime(String time, Date noTimeDate)</t>
+  </si>
+  <si>
+    <t>dateNoTIme</t>
+  </si>
+  <si>
+    <t>2, 12</t>
+  </si>
+  <si>
+    <t>2, 8</t>
+  </si>
+  <si>
+    <t>2, 11</t>
+  </si>
+  <si>
+    <t>3, 8</t>
+  </si>
+  <si>
+    <t>3, 11</t>
+  </si>
+  <si>
+    <t>4, 8</t>
+  </si>
+  <si>
+    <t>4, 11</t>
+  </si>
+  <si>
+    <t>5, 8</t>
+  </si>
+  <si>
+    <t>5, 11</t>
+  </si>
+  <si>
+    <t>2, 13</t>
+  </si>
+  <si>
+    <t>TC04_EC</t>
+  </si>
+  <si>
+    <t>TC01_EC</t>
+  </si>
+  <si>
+    <t>"23:60"</t>
+  </si>
+  <si>
+    <t>01. Tasks</t>
+  </si>
+  <si>
+    <t>Aplicatia cu interfata grafica gestioneaza task-urile unei persoane active. Informatiile sunt preluate dintr-un fisier binar sau text gestionat de catre aplicatie, user ul neputand modifica manual fisierul . Functionalitatile aplicatiei sunt:</t>
   </si>
   <si>
     <r>
@@ -613,56 +642,44 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> combinarea unei date cu a unui timp(time, no</t>
+      <t xml:space="preserve"> . Adaugarea unui task nou cu detaliile: titlul, data si ora de inceput, data si ora de sfarsit. Daca task-ul este repetitiv, atunci se indica intervalul de timp la care se va repeta, dat ca numar de ore si minute. In cazul in care o repetitive a task ului depaseste data de sfarsit, aceasta nu se mai ia in considerare. Task-ul poate fi activ sau nu. Adaugarea se persista in fisier.</t>
     </r>
   </si>
   <si>
-    <t>noTimeDate</t>
-  </si>
-  <si>
-    <t>timpul e valid, 00:00&lt;t&lt;23:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data e valida, 01.01.1970 &lt;date&lt; 31.12.9999  </t>
-  </si>
-  <si>
-    <t>01. date=31.12.1969</t>
-  </si>
-  <si>
-    <t>02. date=01.01.1970</t>
-  </si>
-  <si>
-    <t>03. date=02.01.1970</t>
-  </si>
-  <si>
-    <t>04. date=30.12.9999</t>
-  </si>
-  <si>
-    <t>05. date=31.12.9999</t>
-  </si>
-  <si>
-    <t>06. date=01.01.10000</t>
-  </si>
-  <si>
-    <t>07. time=00:-1</t>
-  </si>
-  <si>
-    <t>08. time=00:00</t>
-  </si>
-  <si>
-    <t>09. time=00:01</t>
-  </si>
-  <si>
-    <t>10. time=23:58</t>
-  </si>
-  <si>
-    <t>11. time=23:59</t>
-  </si>
-  <si>
-    <t>12. time=24:00</t>
-  </si>
-  <si>
-    <t>13. time=23:60</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>F01.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> combinarea unei date cu a unui timp(time, noTimeDate)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">F01. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>combinarea unei date cu a unui timp(time, noTimeDate)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -793,13 +810,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -874,6 +884,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -919,7 +935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1115,30 +1131,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1197,17 +1189,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -1334,6 +1315,82 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1345,7 +1402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1369,10 +1426,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1406,14 +1463,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1423,153 +1474,207 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1577,152 +1682,86 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2031,10 +2070,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,24 +2086,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48"/>
-      <c r="H1" s="43" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="54"/>
+      <c r="H1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2079,10 +2118,10 @@
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="I4" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="40">
         <v>237</v>
       </c>
     </row>
@@ -2090,20 +2129,20 @@
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="29"/>
+      <c r="B6" s="27"/>
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2129,14 +2168,16 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2144,48 +2185,57 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C20" s="39" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2200,47 +2250,30 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
-      <c r="B24" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="45"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C26" s="42"/>
+    <row r="23" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="36"/>
+      <c r="B23" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B24:N24"/>
+    <mergeCell ref="B23:N23"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="H2:J2"/>
   </mergeCells>
@@ -2257,7 +2290,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2275,316 +2308,344 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="G5" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
+      <c r="B5" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="G5" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="G6" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="H6" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="I6" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="J6" s="78"/>
+      <c r="K6" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="59"/>
+      <c r="L6" s="76"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="65" t="s">
-        <v>96</v>
+      <c r="C7" s="56" t="s">
+        <v>76</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="58"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="16" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K7" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="56"/>
+        <v>92</v>
+      </c>
+      <c r="K7" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="79"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="65"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G8" s="16">
         <v>1</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" s="129">
+      <c r="H8" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="44">
         <v>0.4375</v>
       </c>
-      <c r="J8" s="132">
+      <c r="J8" s="46">
         <v>45383</v>
       </c>
-      <c r="K8" s="133">
+      <c r="K8" s="71">
         <v>45383.4375</v>
       </c>
-      <c r="L8" s="52"/>
+      <c r="L8" s="72"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="66" t="s">
-        <v>98</v>
+      <c r="C9" s="64" t="s">
+        <v>78</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="16">
         <v>2</v>
       </c>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="46">
+        <v>45383</v>
+      </c>
+      <c r="K9" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="52"/>
+      <c r="L9" s="72"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="82"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="134">
+        <v>81</v>
+      </c>
+      <c r="G10" s="47">
         <v>3</v>
       </c>
-      <c r="H10" s="135" t="s">
+      <c r="H10" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="62"/>
+      <c r="J10" s="117">
+        <v>45383</v>
+      </c>
+      <c r="K10" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" s="90"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="134">
+        <v>82</v>
+      </c>
+      <c r="G11" s="47">
         <v>4</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="I11" s="130"/>
-      <c r="J11" s="130"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="62"/>
+        <v>91</v>
+      </c>
+      <c r="I11" s="118">
+        <v>1</v>
+      </c>
+      <c r="J11" s="117">
+        <v>45383</v>
+      </c>
+      <c r="K11" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="L11" s="90"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="134"/>
+        <v>86</v>
+      </c>
+      <c r="G12" s="47"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="64"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="68"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="134"/>
+        <v>83</v>
+      </c>
+      <c r="G13" s="47"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="131"/>
-      <c r="J13" s="131"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="64"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="68"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" s="134"/>
+        <v>84</v>
+      </c>
+      <c r="G14" s="47"/>
       <c r="H14" s="13"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="54"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="70"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="67"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="134"/>
+        <v>85</v>
+      </c>
+      <c r="G15" s="47"/>
       <c r="H15" s="13"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="54"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="70"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="126"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="G16" s="134"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="54"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="70"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="65"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="G17" s="134"/>
+      <c r="G17" s="47"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="54"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="70"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="65"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="G18" s="134"/>
+      <c r="G18" s="47"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="54"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="70"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="65"/>
+      <c r="C19" s="56"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="54"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="70"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="65"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
+        <v>36</v>
+      </c>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K15:L15"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C7:C8"/>
@@ -2601,16 +2662,6 @@
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2621,10 +2672,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:R24"/>
+  <dimension ref="B1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2637,416 +2688,384 @@
     <col min="7" max="7" width="9.44140625" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" customWidth="1"/>
-    <col min="18" max="18" width="9.44140625" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="48"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="81" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="121" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-    </row>
-    <row r="6" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+    </row>
+    <row r="6" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="G6" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="73" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="R6" s="79"/>
-    </row>
-    <row r="7" spans="2:18" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="66">
+      <c r="G6" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="91"/>
+      <c r="M6" s="87" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="88"/>
+    </row>
+    <row r="7" spans="2:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="64">
         <v>1</v>
       </c>
-      <c r="C7" s="83" t="s">
-        <v>115</v>
+      <c r="C7" s="81" t="s">
+        <v>94</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="58"/>
+        <v>95</v>
+      </c>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="75"/>
       <c r="K7" s="16" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="R7" s="56"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="82"/>
-      <c r="C8" s="84"/>
+        <v>112</v>
+      </c>
+      <c r="M7" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="79"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="65"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="G8" s="16">
         <v>1</v>
       </c>
-      <c r="H8" s="14">
-        <v>1</v>
+      <c r="H8" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="J8" s="13"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="76"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
-      <c r="C9" s="84"/>
+      <c r="K8" s="120">
+        <v>0</v>
+      </c>
+      <c r="L8" s="117">
+        <v>25569</v>
+      </c>
+      <c r="M8" s="119">
+        <v>25569</v>
+      </c>
+      <c r="N8" s="90"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="65"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="134">
+        <v>97</v>
+      </c>
+      <c r="G9" s="47">
         <v>2</v>
       </c>
-      <c r="H9" s="14">
-        <v>2</v>
-      </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q9" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" s="76"/>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
-      <c r="C10" s="84"/>
+      <c r="H9" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="120">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L9" s="117">
+        <v>25569</v>
+      </c>
+      <c r="M9" s="119">
+        <v>25569.958333333332</v>
+      </c>
+      <c r="N9" s="90"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="65"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="2" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="G10" s="16">
         <v>3</v>
       </c>
-      <c r="H10" s="14">
-        <v>3</v>
-      </c>
-      <c r="I10" s="13"/>
+      <c r="H10" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="M10" s="27">
-        <v>2010</v>
-      </c>
-      <c r="N10" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="P10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q10" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="R10" s="76"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="82"/>
-      <c r="C11" s="84"/>
+      <c r="K10" s="120">
+        <v>0</v>
+      </c>
+      <c r="L10" s="117">
+        <v>25570</v>
+      </c>
+      <c r="M10" s="119">
+        <v>25570</v>
+      </c>
+      <c r="N10" s="90"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="65"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="2" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="G11" s="16">
         <v>4</v>
       </c>
-      <c r="H11" s="14">
-        <v>4</v>
-      </c>
-      <c r="I11" s="13"/>
+      <c r="H11" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="J11" s="13"/>
-      <c r="K11" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="27">
-        <v>2010</v>
-      </c>
-      <c r="N11" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="R11" s="76"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="67"/>
-      <c r="C12" s="85"/>
+      <c r="K11" s="120">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L11" s="117">
+        <v>25570</v>
+      </c>
+      <c r="M11" s="119">
+        <v>25570.999305555557</v>
+      </c>
+      <c r="N11" s="90"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="66"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="2" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="G12" s="16">
         <v>5</v>
       </c>
-      <c r="H12" s="14">
-        <v>5</v>
-      </c>
-      <c r="I12" s="13"/>
+      <c r="H12" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="J12" s="13"/>
-      <c r="K12" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L12" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" s="27">
-        <v>2010</v>
-      </c>
-      <c r="N12" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="O12" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="P12" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q12" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="R12" s="76"/>
-    </row>
-    <row r="13" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="66">
+      <c r="K12" s="120">
+        <v>0</v>
+      </c>
+      <c r="L12" s="117">
+        <v>2958464</v>
+      </c>
+      <c r="M12" s="119">
+        <v>2958464</v>
+      </c>
+      <c r="N12" s="90"/>
+    </row>
+    <row r="13" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="64">
         <v>3</v>
       </c>
-      <c r="C13" s="83" t="s">
-        <v>114</v>
+      <c r="C13" s="81" t="s">
+        <v>93</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="G13" s="16">
         <v>12</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="J13" s="13"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="76"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="82"/>
-      <c r="C14" s="84"/>
+      <c r="K13" s="120">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L13" s="117">
+        <v>2958464</v>
+      </c>
+      <c r="M13" s="119">
+        <v>2958464.9993055556</v>
+      </c>
+      <c r="N13" s="90"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="65"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="2" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="G14" s="16">
         <v>13</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="J14" s="13"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="76"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
-      <c r="C15" s="84"/>
+      <c r="K14" s="120">
+        <v>0</v>
+      </c>
+      <c r="L14" s="117">
+        <v>2958465</v>
+      </c>
+      <c r="M14" s="119">
+        <v>2958465</v>
+      </c>
+      <c r="N14" s="90"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="65"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="2" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="G15" s="16">
         <v>14</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="13"/>
+      <c r="H15" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="J15" s="13"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="76"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
-      <c r="C16" s="84"/>
+      <c r="K15" s="120">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L15" s="117">
+        <v>2958465</v>
+      </c>
+      <c r="M15" s="119">
+        <v>2958465.9993055556</v>
+      </c>
+      <c r="N15" s="90"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="65"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="2" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="G16" s="16">
         <v>15</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="13"/>
+      <c r="H16" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>123</v>
+      </c>
       <c r="J16" s="13"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="75"/>
-      <c r="R16" s="76"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
-      <c r="C17" s="84"/>
+      <c r="K16" s="118">
+        <v>1</v>
+      </c>
+      <c r="L16" s="117">
+        <v>25569</v>
+      </c>
+      <c r="M16" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="N16" s="90"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="65"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="G17" s="16">
         <v>16</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="13"/>
+      <c r="H17" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>123</v>
+      </c>
       <c r="J17" s="13"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="76"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="82"/>
-      <c r="C18" s="84"/>
+      <c r="K17" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" s="117">
+        <v>25569</v>
+      </c>
+      <c r="M17" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="N17" s="90"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="65"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="G18" s="16">
         <v>17</v>
@@ -3054,20 +3073,16 @@
       <c r="H18" s="14"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="76"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="82"/>
-      <c r="C19" s="84"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="90"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="65"/>
+      <c r="C19" s="82"/>
       <c r="D19" s="2" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="G19" s="16">
         <v>18</v>
@@ -3075,86 +3090,78 @@
       <c r="H19" s="14"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="76"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="128"/>
-      <c r="C20" s="136"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="89"/>
+      <c r="N19" s="90"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="43"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="128"/>
-      <c r="C21" s="136"/>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="43"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="128"/>
-      <c r="C22" s="136"/>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="43"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="2"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="80"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="80"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="35"/>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="128"/>
-      <c r="C23" s="136"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="85"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="43"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="2"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="86"/>
-      <c r="N23" s="36"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="127"/>
-      <c r="C24" s="137"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="84"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="42"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M8:N8"/>
     <mergeCell ref="B13:B19"/>
     <mergeCell ref="C13:C19"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="I23:M23"/>
-    <mergeCell ref="G5:R5"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:M22"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3169,15 +3176,15 @@
   </sheetPr>
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
     <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.88671875" customWidth="1"/>
@@ -3186,127 +3193,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="125" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="125"/>
-      <c r="N3" s="125"/>
+      <c r="B3" s="129" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="131"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="119" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="104" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="59"/>
+      <c r="B4" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="114" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="78"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="128" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="103"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="105"/>
-      <c r="E5" s="118"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="19" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="112" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="113"/>
-      <c r="M5" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="17">
         <v>1</v>
       </c>
-      <c r="C6" s="101" t="s">
-        <v>73</v>
+      <c r="C6" s="123" t="s">
+        <v>54</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="22">
-        <v>2010</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="114" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="115" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>43</v>
+        <v>56</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -3314,37 +3283,24 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="101"/>
+      <c r="C7" s="96"/>
       <c r="D7" s="24" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H7" s="8">
-        <v>2010</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="121" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="122"/>
-      <c r="M7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>43</v>
+        <v>56</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -3352,37 +3308,24 @@
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="24" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -3390,37 +3333,24 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="101"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="24" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="123" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="124"/>
-      <c r="M9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -3428,37 +3358,24 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="101"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="G10" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="10">
-        <v>2010</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" s="116" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="117"/>
-      <c r="M10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>43</v>
+        <v>56</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -3466,37 +3383,24 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="101"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="24" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="10">
-        <v>2010</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K11" s="116" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="117"/>
-      <c r="M11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>43</v>
+        <v>56</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -3504,37 +3408,24 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="101"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="24" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="10">
-        <v>2010</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K12" s="116" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="117"/>
-      <c r="M12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>43</v>
+        <v>56</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3542,37 +3433,24 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="102"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="25" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="110" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="111"/>
-      <c r="M13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3592,7 +3470,7 @@
     </row>
     <row r="15" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="20" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
@@ -3602,137 +3480,137 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="100"/>
-      <c r="L15" s="100"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="89" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="89" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="90"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="92"/>
-      <c r="M17" s="89" t="s">
-        <v>86</v>
-      </c>
-      <c r="N17" s="90"/>
-      <c r="O17" s="91"/>
-      <c r="P17" s="92"/>
+      <c r="C17" s="105" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="125" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="126"/>
+      <c r="J17" s="126"/>
+      <c r="K17" s="126"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17" s="108"/>
+      <c r="O17" s="106"/>
+      <c r="P17" s="107"/>
     </row>
     <row r="18" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="101" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="102" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="109" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="87" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="99" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="95" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" s="96"/>
-      <c r="J18" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="K18" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="L18" s="88" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" s="93" t="s">
-        <v>92</v>
-      </c>
-      <c r="N18" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="O18" s="87" t="s">
-        <v>88</v>
-      </c>
-      <c r="P18" s="88" t="s">
-        <v>89</v>
+      <c r="E18" s="103" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="113" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="109" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="110"/>
+      <c r="J18" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="M18" s="114" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" s="103" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="P18" s="104" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="108"/>
-      <c r="C19" s="109"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="97"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="94"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="87"/>
-      <c r="P19" s="88"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="115"/>
+      <c r="N19" s="103"/>
+      <c r="O19" s="103"/>
+      <c r="P19" s="104"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="30">
+      <c r="B20" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="28">
         <v>8</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="30">
         <v>5</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="30">
         <v>3</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="106" t="s">
-        <v>93</v>
-      </c>
-      <c r="I20" s="107"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="100"/>
       <c r="J20" s="2">
         <v>3</v>
       </c>
-      <c r="K20" s="32">
+      <c r="K20" s="30">
         <v>3</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="31">
         <v>0</v>
       </c>
-      <c r="M20" s="37" t="s">
-        <v>93</v>
+      <c r="M20" s="33" t="s">
+        <v>74</v>
       </c>
       <c r="N20" s="2">
         <v>5</v>
       </c>
-      <c r="O20" s="32">
+      <c r="O20" s="30">
         <v>5</v>
       </c>
-      <c r="P20" s="33">
+      <c r="P20" s="31">
         <v>0</v>
       </c>
     </row>
@@ -3740,25 +3618,17 @@
       <c r="M21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="B3:N3"/>
+  <mergeCells count="27">
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
     <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
@@ -3771,12 +3641,11 @@
     <mergeCell ref="H18:I19"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3785,6 +3654,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -3928,22 +3812,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3959,21 +3845,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
modifications to excel, validated by teacher
</commit_message>
<xml_diff>
--- a/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB9143B-65EC-4D49-9E9F-6116DC7D9A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA392BDF-BC79-44DC-A92B-9BB37AF1128C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="125">
   <si>
     <t>VVSS, Info Romana, 2023-2024</t>
   </si>
@@ -435,9 +435,6 @@
     <t>timpul este valid</t>
   </si>
   <si>
-    <t>data este inexistenta (30.02)</t>
-  </si>
-  <si>
     <t>timpul nu contine ":"</t>
   </si>
   <si>
@@ -472,12 +469,6 @@
   </si>
   <si>
     <t>noTimeDate</t>
-  </si>
-  <si>
-    <t>timpul e valid, 00:00&lt;t&lt;23:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data e valida, 01.01.1970 &lt;date&lt; 31.12.9999  </t>
   </si>
   <si>
     <t>01. date=31.12.1969</t>
@@ -661,14 +652,23 @@
     <t>yes</t>
   </si>
   <si>
-    <t>not applicable</t>
+    <t>data este inexistenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data e valida, 01.01.1970 &lt;=date&lt;= 31.12.9999  </t>
+  </si>
+  <si>
+    <t>timpul e valid, 00:00&lt;=t&lt;=23:59</t>
+  </si>
+  <si>
+    <t>no exception thrown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -750,26 +750,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -864,6 +846,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1386,53 +1377,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1442,19 +1431,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1470,16 +1459,16 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1491,19 +1480,19 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1516,33 +1505,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1578,16 +1540,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1599,13 +1567,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1614,126 +1594,141 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2057,24 +2052,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="55"/>
-      <c r="H1" s="35" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
+      <c r="H1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2089,10 +2084,10 @@
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="34">
         <v>237</v>
       </c>
     </row>
@@ -2100,24 +2095,24 @@
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="J5" s="36">
+      <c r="I5" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="34">
         <v>237</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
+      <c r="B6" s="21"/>
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2144,7 +2139,7 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2152,7 +2147,7 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2160,7 +2155,7 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2172,7 +2167,7 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="31" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2182,8 +2177,8 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C19" s="31" t="s">
-        <v>96</v>
+      <c r="C19" s="29" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2226,25 +2221,25 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="52" t="s">
+      <c r="A23" s="30"/>
+      <c r="B23" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C25" s="34"/>
+      <c r="C25" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2265,7 +2260,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:L8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2283,322 +2278,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="67" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="69"/>
+      <c r="B3" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="G5" s="71" t="s">
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="G5" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="61"/>
-      <c r="K6" s="59" t="s">
+      <c r="J6" s="79"/>
+      <c r="K6" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="59"/>
+      <c r="L6" s="77"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="55" t="s">
         <v>61</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="60" t="s">
+      <c r="G7" s="62"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="62"/>
+      <c r="L7" s="80"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="13">
+        <v>121</v>
+      </c>
+      <c r="G8" s="11">
         <v>1</v>
       </c>
-      <c r="H8" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="40">
+      <c r="H8" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="38">
         <v>0.4375</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="40">
         <v>45383</v>
       </c>
-      <c r="K8" s="81">
+      <c r="K8" s="72">
         <v>45383.4375</v>
       </c>
-      <c r="L8" s="82"/>
+      <c r="L8" s="73"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="63" t="s">
         <v>63</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="G9" s="13">
+      <c r="G9" s="11">
         <v>2</v>
       </c>
-      <c r="H9" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="42">
+      <c r="H9" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="40">
         <v>45383</v>
       </c>
-      <c r="K9" s="83" t="s">
-        <v>94</v>
-      </c>
-      <c r="L9" s="82"/>
+      <c r="K9" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="73"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="75"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="43">
+        <v>65</v>
+      </c>
+      <c r="G10" s="41">
         <v>3</v>
       </c>
-      <c r="H10" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J10" s="48">
+      <c r="H10" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="46">
         <v>45383</v>
       </c>
-      <c r="K10" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="L10" s="78"/>
+      <c r="K10" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="67"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="43">
+        <v>66</v>
+      </c>
+      <c r="G11" s="41">
         <v>4</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="49">
+      <c r="H11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="47">
         <v>1</v>
       </c>
-      <c r="J11" s="48">
+      <c r="J11" s="46">
         <v>45383</v>
       </c>
-      <c r="K11" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="L11" s="78"/>
+      <c r="K11" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="67"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="75"/>
+      <c r="C12" s="64"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="80"/>
+        <v>70</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="69"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="75"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="80"/>
+        <v>67</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="69"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="75"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="65"/>
+        <v>68</v>
+      </c>
+      <c r="G14" s="41"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="71"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="76"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="65"/>
+        <v>69</v>
+      </c>
+      <c r="G15" s="41"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="71"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="65"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="71"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="66"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="65"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="71"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="65"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="71"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="66"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="65"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="71"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="66"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -2606,11 +2601,21 @@
       <c r="D22" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K15:L15"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C7:C8"/>
@@ -2627,16 +2632,6 @@
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2650,7 +2645,7 @@
   <dimension ref="B1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2670,40 +2665,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="94" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="69"/>
+      <c r="B3" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
     </row>
     <row r="6" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -2715,404 +2710,406 @@
       <c r="D6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="G6" s="72" t="s">
+      <c r="E6" s="6"/>
+      <c r="G6" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="H6" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="72" t="s">
+      <c r="I6" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="57" t="s">
+      <c r="J6" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="85" t="s">
+      <c r="K6" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="86"/>
-      <c r="M6" s="85" t="s">
+      <c r="L6" s="92"/>
+      <c r="M6" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="93"/>
+      <c r="N6" s="90"/>
     </row>
     <row r="7" spans="2:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="74">
+      <c r="B7" s="63">
         <v>1</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="82" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="80"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="64"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="48">
+        <v>0</v>
+      </c>
+      <c r="L8" s="46">
+        <v>25569</v>
+      </c>
+      <c r="M8" s="91">
+        <v>25569</v>
+      </c>
+      <c r="N8" s="67"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="64"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="G9" s="41">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="48">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L9" s="46">
+        <v>25569</v>
+      </c>
+      <c r="M9" s="91">
+        <v>25569.958333333332</v>
+      </c>
+      <c r="N9" s="67"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="64"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="M7" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="N7" s="62"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="75"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="2" t="s">
+      <c r="G10" s="11">
+        <v>3</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="48">
+        <v>0</v>
+      </c>
+      <c r="L10" s="46">
+        <v>25570</v>
+      </c>
+      <c r="M10" s="91">
+        <v>25570</v>
+      </c>
+      <c r="N10" s="67"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="64"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G11" s="11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="48">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L11" s="46">
+        <v>25570</v>
+      </c>
+      <c r="M11" s="91">
+        <v>25570.999305555557</v>
+      </c>
+      <c r="N11" s="67"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="65"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="11">
+        <v>5</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="48">
+        <v>0</v>
+      </c>
+      <c r="L12" s="46">
+        <v>2958464</v>
+      </c>
+      <c r="M12" s="91">
+        <v>2958464</v>
+      </c>
+      <c r="N12" s="67"/>
+    </row>
+    <row r="13" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="63">
+        <v>3</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="11">
+        <v>12</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="48">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L13" s="46">
+        <v>2958464</v>
+      </c>
+      <c r="M13" s="91">
+        <v>2958464.9993055556</v>
+      </c>
+      <c r="N13" s="67"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="64"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="11">
+        <v>13</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="48">
+        <v>0</v>
+      </c>
+      <c r="L14" s="46">
+        <v>2958465</v>
+      </c>
+      <c r="M14" s="91">
+        <v>2958465</v>
+      </c>
+      <c r="N14" s="67"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="64"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="11">
+        <v>14</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="48">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="L15" s="46">
+        <v>2958465</v>
+      </c>
+      <c r="M15" s="91">
+        <v>2958465.9993055556</v>
+      </c>
+      <c r="N15" s="67"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="64"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="11">
+        <v>15</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="47">
         <v>1</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="50">
-        <v>0</v>
-      </c>
-      <c r="L8" s="48">
+      <c r="L16" s="46">
         <v>25569</v>
       </c>
-      <c r="M8" s="84">
+      <c r="M16" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" s="67"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="64"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="11">
+        <v>16</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L17" s="46">
         <v>25569</v>
       </c>
-      <c r="N8" s="78"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="75"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="43">
-        <v>2</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="50">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="L9" s="48">
-        <v>25569</v>
-      </c>
-      <c r="M9" s="84">
-        <v>25569.958333333332</v>
-      </c>
-      <c r="N9" s="78"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="75"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="13">
-        <v>3</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="50">
-        <v>0</v>
-      </c>
-      <c r="L10" s="48">
-        <v>25570</v>
-      </c>
-      <c r="M10" s="84">
-        <v>25570</v>
-      </c>
-      <c r="N10" s="78"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="75"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="13">
-        <v>4</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="50">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="L11" s="48">
-        <v>25570</v>
-      </c>
-      <c r="M11" s="84">
-        <v>25570.999305555557</v>
-      </c>
-      <c r="N11" s="78"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="76"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="13">
-        <v>5</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="50">
-        <v>0</v>
-      </c>
-      <c r="L12" s="48">
-        <v>2958464</v>
-      </c>
-      <c r="M12" s="84">
-        <v>2958464</v>
-      </c>
-      <c r="N12" s="78"/>
-    </row>
-    <row r="13" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="74">
-        <v>3</v>
-      </c>
-      <c r="C13" s="87" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" s="13">
-        <v>12</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="50">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="L13" s="48">
-        <v>2958464</v>
-      </c>
-      <c r="M13" s="84">
-        <v>2958464.9993055556</v>
-      </c>
-      <c r="N13" s="78"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="75"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="13">
-        <v>13</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="50">
-        <v>0</v>
-      </c>
-      <c r="L14" s="48">
-        <v>2958465</v>
-      </c>
-      <c r="M14" s="84">
-        <v>2958465</v>
-      </c>
-      <c r="N14" s="78"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="75"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="2" t="s">
+      <c r="M17" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="67"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="64"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="13">
-        <v>14</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="50">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="L15" s="48">
-        <v>2958465</v>
-      </c>
-      <c r="M15" s="84">
-        <v>2958465.9993055556</v>
-      </c>
-      <c r="N15" s="78"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="75"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="2" t="s">
+      <c r="G18" s="11">
+        <v>17</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="67"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="64"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="13">
-        <v>15</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="49">
-        <v>1</v>
-      </c>
-      <c r="L16" s="48">
-        <v>25569</v>
-      </c>
-      <c r="M16" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="N16" s="78"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="75"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="13">
-        <v>16</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="L17" s="48">
-        <v>25569</v>
-      </c>
-      <c r="M17" s="77" t="s">
-        <v>94</v>
-      </c>
-      <c r="N17" s="78"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="75"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="13">
-        <v>17</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="77"/>
-      <c r="N18" s="78"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="75"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="13">
+      <c r="G19" s="11">
         <v>18</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="78"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="67"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="39"/>
-      <c r="C20" s="45"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="39"/>
-      <c r="C21" s="45"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="39"/>
-      <c r="C22" s="45"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="2"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="91"/>
-      <c r="L22" s="91"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="39"/>
-      <c r="C23" s="45"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="2"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="90"/>
-      <c r="K23" s="90"/>
-      <c r="L23" s="90"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="38"/>
-      <c r="C24" s="46"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="C13:C19"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
@@ -3129,14 +3126,12 @@
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="C13:C19"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3149,10 +3144,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:P25"/>
+  <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3168,82 +3163,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="127"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="101"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="51" t="s">
+      <c r="G4" s="79"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="49" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="124"/>
-      <c r="C5" s="123"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="16" t="s">
+      <c r="B5" s="98"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="127" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>1</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="38">
         <v>0.4375</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="40">
         <v>45383</v>
       </c>
       <c r="H6" s="128">
@@ -3254,121 +3249,121 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="C7" s="123"/>
+      <c r="D7" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="G7" s="42">
+      <c r="F7" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="40">
         <v>45383</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>122</v>
+      <c r="H7" s="129" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="129" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="123"/>
+      <c r="D8" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="48">
+      <c r="F8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="46">
         <v>45383</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>122</v>
+      <c r="H8" s="129" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="129" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="C9" s="123"/>
+      <c r="D9" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="49">
+      <c r="F9" s="47">
         <v>1</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="46">
         <v>45383</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>122</v>
+      <c r="H9" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="123"/>
+      <c r="D10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="50">
+      <c r="E10" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="48">
         <v>0</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="46">
         <v>25569</v>
       </c>
-      <c r="H10" s="129">
+      <c r="H10" s="130">
         <v>25569</v>
       </c>
-      <c r="I10" s="129">
+      <c r="I10" s="130">
         <v>25569</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="123"/>
+      <c r="D11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="50">
+      <c r="E11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="48">
         <v>0.99930555555555556</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="46">
         <v>25569</v>
       </c>
       <c r="H11" s="130">
@@ -3379,21 +3374,21 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="98"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="123"/>
+      <c r="D12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="48">
         <v>0</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="46">
         <v>25570</v>
       </c>
       <c r="H12" s="130">
@@ -3404,422 +3399,210 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="15">
+      <c r="B13" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="99"/>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="124"/>
+      <c r="D13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="49">
+      <c r="E13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="47">
         <v>1</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="46">
         <v>25569</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>94</v>
+      <c r="H13" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="126" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
     </row>
     <row r="15" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="109"/>
-      <c r="L15" s="109"/>
-      <c r="M15" s="6"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="117"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M16" s="6"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="25" t="s">
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="114" t="s">
+      <c r="H17" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="115"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="104" t="s">
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="N17" s="105"/>
-      <c r="O17" s="106"/>
-      <c r="P17" s="107"/>
+      <c r="N17" s="112"/>
+      <c r="O17" s="113"/>
+      <c r="P17" s="114"/>
     </row>
     <row r="18" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="112" t="s">
+      <c r="B18" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="102" t="s">
+      <c r="E18" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="103" t="s">
+      <c r="F18" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="121" t="s">
+      <c r="G18" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="117" t="s">
+      <c r="H18" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="118"/>
-      <c r="J18" s="72" t="s">
+      <c r="I18" s="107"/>
+      <c r="J18" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="72" t="s">
+      <c r="K18" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="L18" s="100" t="s">
+      <c r="L18" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="M18" s="95" t="s">
+      <c r="M18" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="102" t="s">
+      <c r="N18" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="102" t="s">
+      <c r="O18" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="103" t="s">
+      <c r="P18" s="105" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="112"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="102"/>
-      <c r="F19" s="103"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="119"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="101"/>
-      <c r="M19" s="108"/>
-      <c r="N19" s="102"/>
-      <c r="O19" s="102"/>
-      <c r="P19" s="103"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="105"/>
+      <c r="G19" s="110"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="116"/>
+      <c r="N19" s="104"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="105"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="24">
-        <v>10</v>
-      </c>
-      <c r="D20" s="26">
-        <v>10</v>
-      </c>
-      <c r="E20" s="26">
+      <c r="C20" s="22">
+        <v>8</v>
+      </c>
+      <c r="D20" s="24">
+        <v>7</v>
+      </c>
+      <c r="E20" s="24">
+        <v>1</v>
+      </c>
+      <c r="F20" s="25">
+        <v>2</v>
+      </c>
+      <c r="G20" s="28">
+        <v>2</v>
+      </c>
+      <c r="H20" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="I20" s="94"/>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="25">
+        <v>1</v>
+      </c>
+      <c r="L20" s="25">
         <v>0</v>
       </c>
-      <c r="F20" s="27">
+      <c r="M20" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="N20" s="22">
+        <v>7</v>
+      </c>
+      <c r="O20" s="24">
+        <v>7</v>
+      </c>
+      <c r="P20" s="24">
         <v>0</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="111"/>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="27">
-        <v>0</v>
-      </c>
-      <c r="L20" s="27">
-        <v>0</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="N20" s="24">
-        <v>10</v>
-      </c>
-      <c r="O20" s="26">
-        <v>10</v>
-      </c>
-      <c r="P20" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="24">
-        <v>1</v>
-      </c>
-      <c r="D21" s="26">
-        <v>1</v>
-      </c>
-      <c r="E21" s="26">
-        <v>0</v>
-      </c>
-      <c r="F21" s="27">
-        <v>0</v>
-      </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="111"/>
-      <c r="J21" s="2">
-        <v>0</v>
-      </c>
-      <c r="K21" s="27">
-        <v>0</v>
-      </c>
-      <c r="L21" s="27">
-        <v>0</v>
-      </c>
-      <c r="M21" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="N21" s="24">
-        <v>1</v>
-      </c>
-      <c r="O21" s="26">
-        <v>1</v>
-      </c>
-      <c r="P21" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="24">
-        <v>1</v>
-      </c>
-      <c r="D22" s="26">
-        <v>1</v>
-      </c>
-      <c r="E22" s="26">
-        <v>0</v>
-      </c>
-      <c r="F22" s="27">
-        <v>0</v>
-      </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="111"/>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="27">
-        <v>0</v>
-      </c>
-      <c r="L22" s="27">
-        <v>0</v>
-      </c>
-      <c r="M22" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="N22" s="24">
-        <v>1</v>
-      </c>
-      <c r="O22" s="26">
-        <v>1</v>
-      </c>
-      <c r="P22" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="24">
-        <v>1</v>
-      </c>
-      <c r="D23" s="26">
-        <v>0</v>
-      </c>
-      <c r="E23" s="26">
-        <v>1</v>
-      </c>
-      <c r="F23" s="27">
-        <v>2</v>
-      </c>
-      <c r="G23" s="30">
-        <v>2</v>
-      </c>
-      <c r="H23" s="110" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" s="111"/>
-      <c r="J23" s="2">
-        <v>1</v>
-      </c>
-      <c r="K23" s="26">
-        <v>1</v>
-      </c>
-      <c r="L23" s="27">
-        <v>0</v>
-      </c>
-      <c r="M23" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="N23" s="2">
-        <v>0</v>
-      </c>
-      <c r="O23" s="26">
-        <v>0</v>
-      </c>
-      <c r="P23" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B24" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="26">
-        <v>1</v>
-      </c>
-      <c r="E24" s="26">
-        <v>0</v>
-      </c>
-      <c r="F24" s="27">
-        <v>0</v>
-      </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="111"/>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-      <c r="K24" s="27">
-        <v>0</v>
-      </c>
-      <c r="L24" s="27">
-        <v>0</v>
-      </c>
-      <c r="M24" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="N24" s="24">
-        <v>1</v>
-      </c>
-      <c r="O24" s="26">
-        <v>1</v>
-      </c>
-      <c r="P24" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B25" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="24">
-        <v>8</v>
-      </c>
-      <c r="D25" s="26">
-        <v>8</v>
-      </c>
-      <c r="E25" s="26">
-        <v>0</v>
-      </c>
-      <c r="F25" s="27">
-        <v>0</v>
-      </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="111"/>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-      <c r="K25" s="27">
-        <v>0</v>
-      </c>
-      <c r="L25" s="27">
-        <v>0</v>
-      </c>
-      <c r="M25" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="N25" s="24">
-        <v>1</v>
-      </c>
-      <c r="O25" s="26">
-        <v>1</v>
-      </c>
-      <c r="P25" s="26">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B3:I3"/>
+  <mergeCells count="27">
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="K18:K19"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
@@ -3828,20 +3611,12 @@
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="H18:I19"/>
     <mergeCell ref="G18:G19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B3:I3"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3850,6 +3625,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -3993,22 +3783,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4024,21 +3816,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>